<commit_message>
docs: update project files
Update project files.
</commit_message>
<xml_diff>
--- a/Project-6-360-Video/360 video - the plan.xlsx
+++ b/Project-6-360-Video/360 video - the plan.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
   <si>
     <t>Description</t>
   </si>
@@ -117,9 +117,6 @@
     <t>This will be my friend</t>
   </si>
   <si>
-    <t>+ case of beer</t>
-  </si>
-  <si>
     <t>Movie prop for explosion</t>
   </si>
   <si>
@@ -132,9 +129,6 @@
     <t>I will sweet talk the security desk into letting me film my movie for free</t>
   </si>
   <si>
-    <t>Find a good alley way to shoot the scene</t>
-  </si>
-  <si>
     <t>Fire kit</t>
   </si>
   <si>
@@ -154,6 +148,48 @@
   </si>
   <si>
     <t>* buy from kijiji</t>
+  </si>
+  <si>
+    <t>(6-pack of beer)</t>
+  </si>
+  <si>
+    <t>Pure Glycol</t>
+  </si>
+  <si>
+    <t>Liquid for smoke machine</t>
+  </si>
+  <si>
+    <t>Make-up artist</t>
+  </si>
+  <si>
+    <t>My wife will be preparing the "dead"</t>
+  </si>
+  <si>
+    <t>Make-up kit</t>
+  </si>
+  <si>
+    <t>colors and stuff</t>
+  </si>
+  <si>
+    <t>Clothing for actors and dead people</t>
+  </si>
+  <si>
+    <t>Purchase cheap halloween costumes</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Food for cast</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>Gas for car</t>
+  </si>
+  <si>
+    <t>Find a good alleyway to shoot the scene</t>
   </si>
 </sst>
 </file>
@@ -259,7 +295,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -277,8 +313,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -298,15 +336,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -333,8 +365,19 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -343,6 +386,7 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -351,6 +395,7 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -683,7 +728,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:F34"/>
+  <dimension ref="A2:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -699,12 +744,12 @@
   <sheetData>
     <row r="2" spans="1:6">
       <c r="A2" s="1"/>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
     </row>
     <row r="3" spans="1:6">
       <c r="B3" s="9" t="s">
@@ -723,7 +768,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1"/>
-      <c r="B4" s="18">
+      <c r="B4" s="16">
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -732,26 +777,26 @@
       <c r="D4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="20">
         <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" s="18">
+      <c r="B5" s="16">
         <v>2</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="22">
+        <v>36</v>
+      </c>
+      <c r="E5" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" s="18">
+      <c r="B6" s="16">
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -760,372 +805,462 @@
       <c r="D6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="B7" s="18">
+      <c r="B7" s="16">
         <v>4</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="20">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" s="16">
+        <v>5</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="22">
+      <c r="D8" s="7"/>
+      <c r="E8" s="20">
         <v>0</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1"/>
-      <c r="B8" s="18">
-        <v>5</v>
-      </c>
-      <c r="C8" s="19" t="s">
+      <c r="F8" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1"/>
+      <c r="B9" s="16">
+        <v>6</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="22">
+      <c r="D9" s="6"/>
+      <c r="E9" s="20">
         <v>50</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="4"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15" t="s">
+      <c r="F9" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1"/>
+      <c r="B10" s="16">
+        <v>7</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="4"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="16"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1">
-      <c r="A11" s="4"/>
-      <c r="B11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="14"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="4"/>
-      <c r="B12" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1">
       <c r="A13" s="4"/>
-      <c r="B13" s="8">
-        <v>1</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="20">
-        <v>0</v>
-      </c>
+      <c r="B13" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="4"/>
-      <c r="B14" s="8">
-        <v>2</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="20">
+      <c r="B14" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>0</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="4"/>
       <c r="B15" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="20">
+        <v>19</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="18">
         <v>0</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="4"/>
       <c r="B16" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="20">
+        <v>28</v>
+      </c>
+      <c r="E16" s="18">
         <v>0</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="4"/>
       <c r="B17" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="20">
-        <v>0</v>
+      <c r="E17" s="18">
+        <v>15</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="4"/>
       <c r="B18" s="8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="20">
-        <v>0</v>
+      <c r="E18" s="18">
+        <v>15</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="4"/>
+      <c r="B19" s="8">
+        <v>5</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="18">
+        <v>15</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1">
+      <c r="B20" s="8">
+        <v>6</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="18">
+        <v>15</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="4"/>
-      <c r="B21" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
+      <c r="B21" s="8">
+        <v>7</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="18">
+        <v>100</v>
+      </c>
+      <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="4"/>
-      <c r="B22" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>23</v>
-      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="4"/>
-      <c r="B23" s="8">
-        <v>1</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:6" ht="15" customHeight="1">
       <c r="A24" s="4"/>
-      <c r="B24" s="8">
-        <v>2</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24" s="20">
-        <v>20</v>
-      </c>
+      <c r="B24" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="4"/>
-      <c r="B25" s="8">
+      <c r="B25" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="20">
-        <v>20</v>
+      <c r="C25" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="4"/>
-      <c r="B26" s="8">
-        <v>4</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E26" s="20">
-        <v>10</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>42</v>
+      <c r="B26" s="26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="28">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="4"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="16"/>
+      <c r="B27" s="26">
+        <v>2</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="28">
+        <v>20</v>
+      </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1">
+      <c r="B28" s="26">
+        <v>3</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" s="28">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="4"/>
-      <c r="B29" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
+      <c r="B29" s="26">
+        <v>4</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="4"/>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="26">
+        <v>5</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="4"/>
+      <c r="B31" s="26">
+        <v>6</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="4"/>
+      <c r="B32" s="26">
+        <v>7</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" s="18">
+        <v>10</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="4"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="13"/>
+      <c r="E33" s="14"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" ht="15" customHeight="1">
+      <c r="A35" s="4"/>
+      <c r="B35" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="4"/>
+      <c r="B36" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C36" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D36" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E36" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="75">
-      <c r="A31" s="4"/>
-      <c r="B31" s="8">
+    <row r="37" spans="1:5" ht="75">
+      <c r="A37" s="4"/>
+      <c r="B37" s="8">
         <v>1</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C37" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" s="23">
+      <c r="D37" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="5"/>
-      <c r="B32" s="17">
+    <row r="38" spans="1:5">
+      <c r="A38" s="5"/>
+      <c r="B38" s="15">
         <v>2</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C38" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D38" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E38" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="C39" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="D40" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="E32" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="3:5">
-      <c r="C33" s="21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="3:5">
-      <c r="D34" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="E34" s="25">
-        <f>SUM(E4:E8)+SUM(E13:E18)+SUM(E23:E26)+SUM(E31:E32)</f>
-        <v>400</v>
+      <c r="E40" s="23">
+        <f>SUM(E4:E10)+SUM(E15:E21)+SUM(E26:E32)+SUM(E37:E38)</f>
+        <v>700</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B35:E35"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>